<commit_message>
finalize virtual booking conversion method
</commit_message>
<xml_diff>
--- a/virtual-bookings.xlsx
+++ b/virtual-bookings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrosenberg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D378A20-139F-4080-AC3F-32EDAF1B7DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7F3AB00-FAD9-474A-A494-561AC12ED798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="24000" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="5820" windowWidth="24000" windowHeight="15440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoices" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="738">
   <si>
     <t>Start Date</t>
   </si>
@@ -1921,9 +1921,6 @@
     <t>SIE Film Center</t>
   </si>
   <si>
-    <t>Time &amp; Space Ltd.</t>
-  </si>
-  <si>
     <t>Davis Varsity</t>
   </si>
   <si>
@@ -2023,9 +2020,6 @@
     <t>Grand Illusion Cinema</t>
   </si>
   <si>
-    <t>The Strand Theatre</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cinematique Theater </t>
   </si>
   <si>
@@ -2053,9 +2047,6 @@
     <t>The Plaza Theatre</t>
   </si>
   <si>
-    <t>Dairy Center for the Arts</t>
-  </si>
-  <si>
     <t>PAC Film House</t>
   </si>
   <si>
@@ -2110,9 +2101,6 @@
     <t>The Cinema Theater</t>
   </si>
   <si>
-    <t>Music Box</t>
-  </si>
-  <si>
     <t>Jean Cocteau Cinema</t>
   </si>
   <si>
@@ -2185,9 +2173,6 @@
     <t>Olympia Film Society</t>
   </si>
   <si>
-    <t>Future of Film is Female STREAMING</t>
-  </si>
-  <si>
     <t>ACME Screening Room</t>
   </si>
   <si>
@@ -2234,6 +2219,24 @@
   </si>
   <si>
     <t xml:space="preserve">Metro Cinema </t>
+  </si>
+  <si>
+    <t>Gateway Film Center 8</t>
+  </si>
+  <si>
+    <t>SIE FilmCenter</t>
+  </si>
+  <si>
+    <t>Time &amp; Space Limited</t>
+  </si>
+  <si>
+    <t>The Dairy Center for the Arts</t>
+  </si>
+  <si>
+    <t>Music Box Theatre</t>
+  </si>
+  <si>
+    <t>Future of Film is Female</t>
   </si>
 </sst>
 </file>
@@ -2602,14 +2605,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D242" sqref="D242"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="D211" sqref="D211"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -2645,7 +2648,7 @@
     <col min="36" max="36" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>44043</v>
       </c>
@@ -2847,7 +2850,7 @@
         <v>7974</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>44043</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>9099</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>44043</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>9204</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>44043</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>9254</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>44043</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>9255</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>44043</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>9256</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>44043</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>9260</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>44043</v>
       </c>
@@ -3299,7 +3302,7 @@
         <v>9261</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>44043</v>
       </c>
@@ -3364,7 +3367,7 @@
         <v>9262</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>44043</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>9265</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>44043</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>9271</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>44043</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>9272</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>44043</v>
       </c>
@@ -3630,7 +3633,7 @@
         <v>9278</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>44043</v>
       </c>
@@ -3695,7 +3698,7 @@
         <v>9279</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>44043</v>
       </c>
@@ -3760,7 +3763,7 @@
         <v>9289</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>44043</v>
       </c>
@@ -3825,7 +3828,7 @@
         <v>9292</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>44043</v>
       </c>
@@ -3890,7 +3893,7 @@
         <v>9293</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>44043</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>625</v>
+        <v>732</v>
       </c>
       <c r="E19" t="s">
         <v>612</v>
@@ -3955,7 +3958,7 @@
         <v>9295</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>44050</v>
       </c>
@@ -4045,7 +4048,7 @@
         <v>9298</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>44050</v>
       </c>
@@ -4110,7 +4113,7 @@
         <v>9302</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
         <v>44043</v>
       </c>
@@ -4175,7 +4178,7 @@
         <v>9303</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
         <v>44043</v>
       </c>
@@ -4240,7 +4243,7 @@
         <v>9306</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
         <v>44043</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>9324</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
         <v>44043</v>
       </c>
@@ -4370,7 +4373,7 @@
         <v>9326</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
         <v>44050</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>631</v>
+        <v>733</v>
       </c>
       <c r="E26" t="s">
         <v>612</v>
@@ -4432,7 +4435,7 @@
         <v>9329</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
         <v>44057</v>
       </c>
@@ -4443,7 +4446,7 @@
         <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>632</v>
+        <v>734</v>
       </c>
       <c r="E27" t="s">
         <v>612</v>
@@ -4494,7 +4497,7 @@
         <v>9336</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
         <v>44043</v>
       </c>
@@ -4505,7 +4508,7 @@
         <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E28" t="s">
         <v>612</v>
@@ -4559,7 +4562,7 @@
         <v>9338</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
         <v>44043</v>
       </c>
@@ -4570,7 +4573,7 @@
         <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E29" t="s">
         <v>612</v>
@@ -4624,7 +4627,7 @@
         <v>9339</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
         <v>44043</v>
       </c>
@@ -4635,7 +4638,7 @@
         <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E30" t="s">
         <v>612</v>
@@ -4662,7 +4665,7 @@
         <v>96</v>
       </c>
       <c r="X30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="Y30" t="s">
         <v>157</v>
@@ -4683,7 +4686,7 @@
         <v>9344</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
         <v>44043</v>
       </c>
@@ -4694,7 +4697,7 @@
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E31" t="s">
         <v>612</v>
@@ -4748,7 +4751,7 @@
         <v>9346</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>44043</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E32" t="s">
         <v>612</v>
@@ -4813,7 +4816,7 @@
         <v>9347</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>44043</v>
       </c>
@@ -4878,7 +4881,7 @@
         <v>9348</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>44043</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>9350</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>43980</v>
       </c>
@@ -4960,7 +4963,7 @@
         <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E35" t="s">
         <v>612</v>
@@ -5020,7 +5023,7 @@
         <v>9043</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>43980</v>
       </c>
@@ -5031,7 +5034,7 @@
         <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E36" t="s">
         <v>612</v>
@@ -5085,7 +5088,7 @@
         <v>9044</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>44008</v>
       </c>
@@ -5096,7 +5099,7 @@
         <v>166</v>
       </c>
       <c r="D37" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E37" t="s">
         <v>612</v>
@@ -5150,7 +5153,7 @@
         <v>9077</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>43987</v>
       </c>
@@ -5161,7 +5164,7 @@
         <v>265</v>
       </c>
       <c r="D38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E38" t="s">
         <v>612</v>
@@ -5215,7 +5218,7 @@
         <v>9097</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>43994</v>
       </c>
@@ -5226,7 +5229,7 @@
         <v>265</v>
       </c>
       <c r="D39" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E39" t="s">
         <v>612</v>
@@ -5280,7 +5283,7 @@
         <v>9126</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>44036</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>9142</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>44029</v>
       </c>
@@ -5380,7 +5383,7 @@
         <v>265</v>
       </c>
       <c r="D41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E41" t="s">
         <v>612</v>
@@ -5434,7 +5437,7 @@
         <v>9264</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>44029</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>265</v>
       </c>
       <c r="D42" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E42" t="s">
         <v>612</v>
@@ -5502,7 +5505,7 @@
         <v>9290</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>44043</v>
       </c>
@@ -5513,7 +5516,7 @@
         <v>265</v>
       </c>
       <c r="D43" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E43" t="s">
         <v>612</v>
@@ -5567,7 +5570,7 @@
         <v>9342</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>44070</v>
       </c>
@@ -5662,7 +5665,7 @@
         <v>9299</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>44121</v>
       </c>
@@ -5751,7 +5754,7 @@
         <v>8876</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>43998</v>
       </c>
@@ -5762,7 +5765,7 @@
         <v>245</v>
       </c>
       <c r="D46" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E46" t="s">
         <v>612</v>
@@ -5816,7 +5819,7 @@
         <v>9082</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>44029</v>
       </c>
@@ -5884,7 +5887,7 @@
         <v>9144</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>44029</v>
       </c>
@@ -5895,7 +5898,7 @@
         <v>245</v>
       </c>
       <c r="D48" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E48" t="s">
         <v>612</v>
@@ -5952,7 +5955,7 @@
         <v>9145</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>44029</v>
       </c>
@@ -5963,7 +5966,7 @@
         <v>245</v>
       </c>
       <c r="D49" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E49" t="s">
         <v>612</v>
@@ -6020,7 +6023,7 @@
         <v>9146</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>44029</v>
       </c>
@@ -6031,7 +6034,7 @@
         <v>245</v>
       </c>
       <c r="D50" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E50" t="s">
         <v>612</v>
@@ -6085,7 +6088,7 @@
         <v>9185</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>44029</v>
       </c>
@@ -6150,7 +6153,7 @@
         <v>9197</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>44029</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>245</v>
       </c>
       <c r="D52" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E52" t="s">
         <v>612</v>
@@ -6215,7 +6218,7 @@
         <v>9205</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>44029</v>
       </c>
@@ -6280,7 +6283,7 @@
         <v>9207</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>44029</v>
       </c>
@@ -6291,7 +6294,7 @@
         <v>245</v>
       </c>
       <c r="D54" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E54" t="s">
         <v>612</v>
@@ -6345,7 +6348,7 @@
         <v>9241</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A55" s="1">
         <v>44029</v>
       </c>
@@ -6356,7 +6359,7 @@
         <v>245</v>
       </c>
       <c r="D55" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E55" t="s">
         <v>612</v>
@@ -6410,7 +6413,7 @@
         <v>9247</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
         <v>44029</v>
       </c>
@@ -6421,7 +6424,7 @@
         <v>245</v>
       </c>
       <c r="D56" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E56" t="s">
         <v>612</v>
@@ -6475,7 +6478,7 @@
         <v>9248</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
         <v>44029</v>
       </c>
@@ -6540,7 +6543,7 @@
         <v>9249</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A58" s="1">
         <v>44029</v>
       </c>
@@ -6551,7 +6554,7 @@
         <v>245</v>
       </c>
       <c r="D58" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E58" t="s">
         <v>612</v>
@@ -6605,7 +6608,7 @@
         <v>9251</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A59" s="1">
         <v>44029</v>
       </c>
@@ -6616,7 +6619,7 @@
         <v>245</v>
       </c>
       <c r="D59" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E59" t="s">
         <v>612</v>
@@ -6670,7 +6673,7 @@
         <v>9252</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A60" s="1">
         <v>44029</v>
       </c>
@@ -6681,7 +6684,7 @@
         <v>245</v>
       </c>
       <c r="D60" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E60" t="s">
         <v>612</v>
@@ -6735,7 +6738,7 @@
         <v>9253</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A61" s="1">
         <v>44029</v>
       </c>
@@ -6746,7 +6749,7 @@
         <v>245</v>
       </c>
       <c r="D61" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E61" t="s">
         <v>612</v>
@@ -6800,7 +6803,7 @@
         <v>9263</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
         <v>44029</v>
       </c>
@@ -6865,7 +6868,7 @@
         <v>9266</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A63" s="1">
         <v>44029</v>
       </c>
@@ -6876,7 +6879,7 @@
         <v>245</v>
       </c>
       <c r="D63" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E63" t="s">
         <v>612</v>
@@ -6930,7 +6933,7 @@
         <v>9268</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A64" s="1">
         <v>44029</v>
       </c>
@@ -6941,7 +6944,7 @@
         <v>245</v>
       </c>
       <c r="D64" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E64" t="s">
         <v>612</v>
@@ -6995,7 +6998,7 @@
         <v>9269</v>
       </c>
     </row>
-    <row r="65" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A65" s="1">
         <v>44029</v>
       </c>
@@ -7006,7 +7009,7 @@
         <v>245</v>
       </c>
       <c r="D65" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E65" t="s">
         <v>612</v>
@@ -7060,7 +7063,7 @@
         <v>9270</v>
       </c>
     </row>
-    <row r="66" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A66" s="1">
         <v>44029</v>
       </c>
@@ -7071,7 +7074,7 @@
         <v>245</v>
       </c>
       <c r="D66" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E66" t="s">
         <v>612</v>
@@ -7125,7 +7128,7 @@
         <v>9273</v>
       </c>
     </row>
-    <row r="67" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
         <v>44029</v>
       </c>
@@ -7190,7 +7193,7 @@
         <v>9277</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A68" s="1">
         <v>44029</v>
       </c>
@@ -7255,7 +7258,7 @@
         <v>9282</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A69" s="1">
         <v>44029</v>
       </c>
@@ -7266,7 +7269,7 @@
         <v>245</v>
       </c>
       <c r="D69" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E69" t="s">
         <v>612</v>
@@ -7320,7 +7323,7 @@
         <v>9284</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A70" s="1">
         <v>44029</v>
       </c>
@@ -7385,7 +7388,7 @@
         <v>9285</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A71" s="1">
         <v>44029</v>
       </c>
@@ -7396,7 +7399,7 @@
         <v>245</v>
       </c>
       <c r="D71" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E71" t="s">
         <v>612</v>
@@ -7450,7 +7453,7 @@
         <v>9288</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
         <v>44036</v>
       </c>
@@ -7515,7 +7518,7 @@
         <v>9305</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A73" s="1">
         <v>44050</v>
       </c>
@@ -7526,7 +7529,7 @@
         <v>245</v>
       </c>
       <c r="D73" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E73" t="s">
         <v>612</v>
@@ -7580,7 +7583,7 @@
         <v>9316</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A74" s="1">
         <v>44084</v>
       </c>
@@ -7672,7 +7675,7 @@
         <v>9318</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>44036</v>
       </c>
@@ -7683,7 +7686,7 @@
         <v>245</v>
       </c>
       <c r="D75" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="E75" t="s">
         <v>612</v>
@@ -7737,7 +7740,7 @@
         <v>9319</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>44036</v>
       </c>
@@ -7748,7 +7751,7 @@
         <v>245</v>
       </c>
       <c r="D76" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E76" t="s">
         <v>612</v>
@@ -7802,7 +7805,7 @@
         <v>9322</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>44043</v>
       </c>
@@ -7861,13 +7864,13 @@
         <v>0</v>
       </c>
       <c r="AI77" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AJ77" s="2">
         <v>9328</v>
       </c>
     </row>
-    <row r="78" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>44043</v>
       </c>
@@ -7878,7 +7881,7 @@
         <v>245</v>
       </c>
       <c r="D78" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E78" t="s">
         <v>612</v>
@@ -7932,7 +7935,7 @@
         <v>9337</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>44043</v>
       </c>
@@ -7943,7 +7946,7 @@
         <v>245</v>
       </c>
       <c r="D79" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E79" t="s">
         <v>612</v>
@@ -7997,7 +8000,7 @@
         <v>9341</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>43966</v>
       </c>
@@ -8062,7 +8065,7 @@
         <v>8742</v>
       </c>
     </row>
-    <row r="81" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>43980</v>
       </c>
@@ -8073,7 +8076,7 @@
         <v>93</v>
       </c>
       <c r="D81" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E81" t="s">
         <v>612</v>
@@ -8127,7 +8130,7 @@
         <v>9013</v>
       </c>
     </row>
-    <row r="82" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>43973</v>
       </c>
@@ -8138,7 +8141,7 @@
         <v>93</v>
       </c>
       <c r="D82" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E82" t="s">
         <v>612</v>
@@ -8192,7 +8195,7 @@
         <v>9014</v>
       </c>
     </row>
-    <row r="83" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
         <v>43973</v>
       </c>
@@ -8203,7 +8206,7 @@
         <v>93</v>
       </c>
       <c r="D83" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E83" t="s">
         <v>612</v>
@@ -8263,7 +8266,7 @@
         <v>9023</v>
       </c>
     </row>
-    <row r="84" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
         <v>43978</v>
       </c>
@@ -8274,7 +8277,7 @@
         <v>93</v>
       </c>
       <c r="D84" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E84" t="s">
         <v>612</v>
@@ -8328,7 +8331,7 @@
         <v>9024</v>
       </c>
     </row>
-    <row r="85" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
         <v>43980</v>
       </c>
@@ -8339,7 +8342,7 @@
         <v>93</v>
       </c>
       <c r="D85" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E85" t="s">
         <v>612</v>
@@ -8393,7 +8396,7 @@
         <v>9036</v>
       </c>
     </row>
-    <row r="86" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
         <v>43980</v>
       </c>
@@ -8404,7 +8407,7 @@
         <v>93</v>
       </c>
       <c r="D86" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E86" t="s">
         <v>612</v>
@@ -8458,7 +8461,7 @@
         <v>9042</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
         <v>43980</v>
       </c>
@@ -8469,7 +8472,7 @@
         <v>93</v>
       </c>
       <c r="D87" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E87" t="s">
         <v>612</v>
@@ -8523,7 +8526,7 @@
         <v>9047</v>
       </c>
     </row>
-    <row r="88" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
         <v>43980</v>
       </c>
@@ -8534,7 +8537,7 @@
         <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E88" t="s">
         <v>612</v>
@@ -8594,7 +8597,7 @@
         <v>9058</v>
       </c>
     </row>
-    <row r="89" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
         <v>43983</v>
       </c>
@@ -8605,7 +8608,7 @@
         <v>93</v>
       </c>
       <c r="D89" t="s">
-        <v>676</v>
+        <v>735</v>
       </c>
       <c r="E89" t="s">
         <v>612</v>
@@ -8659,7 +8662,7 @@
         <v>9061</v>
       </c>
     </row>
-    <row r="90" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
         <v>43987</v>
       </c>
@@ -8670,7 +8673,7 @@
         <v>93</v>
       </c>
       <c r="D90" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E90" t="s">
         <v>612</v>
@@ -8724,7 +8727,7 @@
         <v>9062</v>
       </c>
     </row>
-    <row r="91" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
         <v>43987</v>
       </c>
@@ -8789,7 +8792,7 @@
         <v>9083</v>
       </c>
     </row>
-    <row r="92" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
         <v>44008</v>
       </c>
@@ -8854,7 +8857,7 @@
         <v>9101</v>
       </c>
     </row>
-    <row r="93" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
         <v>43992</v>
       </c>
@@ -8865,7 +8868,7 @@
         <v>93</v>
       </c>
       <c r="D93" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E93" t="s">
         <v>612</v>
@@ -8925,7 +8928,7 @@
         <v>9104</v>
       </c>
     </row>
-    <row r="94" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
         <v>43994</v>
       </c>
@@ -8984,7 +8987,7 @@
         <v>9119</v>
       </c>
     </row>
-    <row r="95" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
         <v>44008</v>
       </c>
@@ -8995,7 +8998,7 @@
         <v>93</v>
       </c>
       <c r="D95" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E95" t="s">
         <v>612</v>
@@ -9040,7 +9043,7 @@
         <v>9174</v>
       </c>
     </row>
-    <row r="96" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
         <v>44043</v>
       </c>
@@ -9105,7 +9108,7 @@
         <v>9345</v>
       </c>
     </row>
-    <row r="97" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
         <v>43973</v>
       </c>
@@ -9116,7 +9119,7 @@
         <v>129</v>
       </c>
       <c r="D97" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E97" t="s">
         <v>612</v>
@@ -9176,7 +9179,7 @@
         <v>9020</v>
       </c>
     </row>
-    <row r="98" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
         <v>43973</v>
       </c>
@@ -9187,7 +9190,7 @@
         <v>129</v>
       </c>
       <c r="D98" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E98" t="s">
         <v>612</v>
@@ -9235,13 +9238,13 @@
         <v>0</v>
       </c>
       <c r="AI98" s="4" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="AJ98" s="2">
         <v>9025</v>
       </c>
     </row>
-    <row r="99" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
         <v>43980</v>
       </c>
@@ -9252,7 +9255,7 @@
         <v>129</v>
       </c>
       <c r="D99" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E99" t="s">
         <v>612</v>
@@ -9306,7 +9309,7 @@
         <v>9037</v>
       </c>
     </row>
-    <row r="100" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
         <v>43987</v>
       </c>
@@ -9371,7 +9374,7 @@
         <v>9084</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
         <v>44022</v>
       </c>
@@ -9382,7 +9385,7 @@
         <v>129</v>
       </c>
       <c r="D101" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E101" t="s">
         <v>612</v>
@@ -9436,7 +9439,7 @@
         <v>9245</v>
       </c>
     </row>
-    <row r="102" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
         <v>44112</v>
       </c>
@@ -9534,7 +9537,7 @@
         <v>9164</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
         <v>44036</v>
       </c>
@@ -9599,7 +9602,7 @@
         <v>9032</v>
       </c>
     </row>
-    <row r="104" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
         <v>44015</v>
       </c>
@@ -9670,7 +9673,7 @@
         <v>9102</v>
       </c>
     </row>
-    <row r="105" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
         <v>44097</v>
       </c>
@@ -9759,7 +9762,7 @@
         <v>8069</v>
       </c>
     </row>
-    <row r="106" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
         <v>44074</v>
       </c>
@@ -9851,7 +9854,7 @@
         <v>9163</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
         <v>44001</v>
       </c>
@@ -9862,7 +9865,7 @@
         <v>233</v>
       </c>
       <c r="D107" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E107" t="s">
         <v>612</v>
@@ -9916,7 +9919,7 @@
         <v>9076</v>
       </c>
     </row>
-    <row r="108" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
         <v>44043</v>
       </c>
@@ -10005,7 +10008,7 @@
         <v>9349</v>
       </c>
     </row>
-    <row r="109" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
         <v>44307</v>
       </c>
@@ -10100,7 +10103,7 @@
         <v>7953</v>
       </c>
     </row>
-    <row r="110" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
         <v>44073</v>
       </c>
@@ -10189,7 +10192,7 @@
         <v>9332</v>
       </c>
     </row>
-    <row r="111" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A111" s="1">
         <v>44008</v>
       </c>
@@ -10254,7 +10257,7 @@
         <v>9030</v>
       </c>
     </row>
-    <row r="112" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A112" s="1">
         <v>44022</v>
       </c>
@@ -10265,7 +10268,7 @@
         <v>149</v>
       </c>
       <c r="D112" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E112" t="s">
         <v>612</v>
@@ -10319,7 +10322,7 @@
         <v>9183</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A113" s="1">
         <v>43973</v>
       </c>
@@ -10330,7 +10333,7 @@
         <v>126</v>
       </c>
       <c r="D113" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E113" t="s">
         <v>612</v>
@@ -10384,7 +10387,7 @@
         <v>9019</v>
       </c>
     </row>
-    <row r="114" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A114" s="1">
         <v>43973</v>
       </c>
@@ -10395,7 +10398,7 @@
         <v>126</v>
       </c>
       <c r="D114" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E114" t="s">
         <v>612</v>
@@ -10455,7 +10458,7 @@
         <v>9021</v>
       </c>
     </row>
-    <row r="115" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A115" s="1">
         <v>43980</v>
       </c>
@@ -10466,7 +10469,7 @@
         <v>126</v>
       </c>
       <c r="D115" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E115" t="s">
         <v>612</v>
@@ -10520,7 +10523,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A116" s="1">
         <v>43987</v>
       </c>
@@ -10585,7 +10588,7 @@
         <v>9085</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A117" s="1">
         <v>44022</v>
       </c>
@@ -10596,7 +10599,7 @@
         <v>126</v>
       </c>
       <c r="D117" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E117" t="s">
         <v>612</v>
@@ -10650,7 +10653,7 @@
         <v>9244</v>
       </c>
     </row>
-    <row r="118" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A118" s="1">
         <v>43973</v>
       </c>
@@ -10661,7 +10664,7 @@
         <v>135</v>
       </c>
       <c r="D118" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E118" t="s">
         <v>612</v>
@@ -10721,7 +10724,7 @@
         <v>9022</v>
       </c>
     </row>
-    <row r="119" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A119" s="1">
         <v>43973</v>
       </c>
@@ -10732,7 +10735,7 @@
         <v>135</v>
       </c>
       <c r="D119" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E119" t="s">
         <v>612</v>
@@ -10786,7 +10789,7 @@
         <v>9026</v>
       </c>
     </row>
-    <row r="120" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A120" s="1">
         <v>43980</v>
       </c>
@@ -10797,7 +10800,7 @@
         <v>135</v>
       </c>
       <c r="D120" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E120" t="s">
         <v>612</v>
@@ -10851,7 +10854,7 @@
         <v>9039</v>
       </c>
     </row>
-    <row r="121" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A121" s="1">
         <v>43987</v>
       </c>
@@ -10916,7 +10919,7 @@
         <v>9086</v>
       </c>
     </row>
-    <row r="122" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A122" s="1">
         <v>44022</v>
       </c>
@@ -10927,7 +10930,7 @@
         <v>135</v>
       </c>
       <c r="D122" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E122" t="s">
         <v>612</v>
@@ -10981,7 +10984,7 @@
         <v>9246</v>
       </c>
     </row>
-    <row r="123" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A123" s="1">
         <v>44036</v>
       </c>
@@ -10992,7 +10995,7 @@
         <v>135</v>
       </c>
       <c r="D123" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E123" t="s">
         <v>612</v>
@@ -11046,7 +11049,7 @@
         <v>9314</v>
       </c>
     </row>
-    <row r="124" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A124" s="1">
         <v>44036</v>
       </c>
@@ -11057,7 +11060,7 @@
         <v>135</v>
       </c>
       <c r="D124" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="E124" t="s">
         <v>612</v>
@@ -11111,7 +11114,7 @@
         <v>9323</v>
       </c>
     </row>
-    <row r="125" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A125" s="1">
         <v>43994</v>
       </c>
@@ -11122,7 +11125,7 @@
         <v>214</v>
       </c>
       <c r="D125" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E125" t="s">
         <v>612</v>
@@ -11176,7 +11179,7 @@
         <v>9064</v>
       </c>
     </row>
-    <row r="126" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A126" s="1">
         <v>43994</v>
       </c>
@@ -11187,7 +11190,7 @@
         <v>112</v>
       </c>
       <c r="D126" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E126" t="s">
         <v>612</v>
@@ -11241,7 +11244,7 @@
         <v>9012</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A127" s="1">
         <v>43994</v>
       </c>
@@ -11252,7 +11255,7 @@
         <v>112</v>
       </c>
       <c r="D127" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E127" t="s">
         <v>612</v>
@@ -11306,7 +11309,7 @@
         <v>9048</v>
       </c>
     </row>
-    <row r="128" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A128" s="1">
         <v>43994</v>
       </c>
@@ -11371,7 +11374,7 @@
         <v>9049</v>
       </c>
     </row>
-    <row r="129" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A129" s="1">
         <v>43994</v>
       </c>
@@ -11439,7 +11442,7 @@
         <v>9050</v>
       </c>
     </row>
-    <row r="130" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A130" s="1">
         <v>47653</v>
       </c>
@@ -11450,7 +11453,7 @@
         <v>112</v>
       </c>
       <c r="D130" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="E130" t="s">
         <v>612</v>
@@ -11504,7 +11507,7 @@
         <v>9051</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A131" s="1">
         <v>43994</v>
       </c>
@@ -11515,7 +11518,7 @@
         <v>112</v>
       </c>
       <c r="D131" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="E131" t="s">
         <v>612</v>
@@ -11569,7 +11572,7 @@
         <v>9053</v>
       </c>
     </row>
-    <row r="132" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A132" s="1">
         <v>43994</v>
       </c>
@@ -11580,7 +11583,7 @@
         <v>112</v>
       </c>
       <c r="D132" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E132" t="s">
         <v>612</v>
@@ -11634,7 +11637,7 @@
         <v>9055</v>
       </c>
     </row>
-    <row r="133" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A133" s="1">
         <v>43994</v>
       </c>
@@ -11645,7 +11648,7 @@
         <v>112</v>
       </c>
       <c r="D133" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E133" t="s">
         <v>612</v>
@@ -11705,7 +11708,7 @@
         <v>9056</v>
       </c>
     </row>
-    <row r="134" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A134" s="1">
         <v>43994</v>
       </c>
@@ -11716,7 +11719,7 @@
         <v>112</v>
       </c>
       <c r="D134" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E134" t="s">
         <v>612</v>
@@ -11776,7 +11779,7 @@
         <v>9059</v>
       </c>
     </row>
-    <row r="135" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A135" s="1">
         <v>43994</v>
       </c>
@@ -11787,7 +11790,7 @@
         <v>112</v>
       </c>
       <c r="D135" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="E135" t="s">
         <v>612</v>
@@ -11841,7 +11844,7 @@
         <v>9060</v>
       </c>
     </row>
-    <row r="136" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A136" s="1">
         <v>43994</v>
       </c>
@@ -11852,7 +11855,7 @@
         <v>112</v>
       </c>
       <c r="D136" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E136" t="s">
         <v>612</v>
@@ -11906,7 +11909,7 @@
         <v>9063</v>
       </c>
     </row>
-    <row r="137" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A137" s="1">
         <v>43994</v>
       </c>
@@ -11917,7 +11920,7 @@
         <v>112</v>
       </c>
       <c r="D137" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E137" t="s">
         <v>612</v>
@@ -11971,7 +11974,7 @@
         <v>9065</v>
       </c>
     </row>
-    <row r="138" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A138" s="1">
         <v>44008</v>
       </c>
@@ -11982,7 +11985,7 @@
         <v>112</v>
       </c>
       <c r="D138" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="E138" t="s">
         <v>612</v>
@@ -12036,7 +12039,7 @@
         <v>9066</v>
       </c>
     </row>
-    <row r="139" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A139" s="1">
         <v>43994</v>
       </c>
@@ -12047,7 +12050,7 @@
         <v>112</v>
       </c>
       <c r="D139" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E139" t="s">
         <v>612</v>
@@ -12101,7 +12104,7 @@
         <v>9067</v>
       </c>
     </row>
-    <row r="140" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A140" s="1">
         <v>43994</v>
       </c>
@@ -12166,7 +12169,7 @@
         <v>9071</v>
       </c>
     </row>
-    <row r="141" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A141" s="1">
         <v>43994</v>
       </c>
@@ -12237,7 +12240,7 @@
         <v>9072</v>
       </c>
     </row>
-    <row r="142" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A142" s="1">
         <v>43994</v>
       </c>
@@ -12248,7 +12251,7 @@
         <v>112</v>
       </c>
       <c r="D142" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E142" t="s">
         <v>612</v>
@@ -12302,7 +12305,7 @@
         <v>9073</v>
       </c>
     </row>
-    <row r="143" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A143" s="1">
         <v>43994</v>
       </c>
@@ -12313,7 +12316,7 @@
         <v>112</v>
       </c>
       <c r="D143" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E143" t="s">
         <v>612</v>
@@ -12367,7 +12370,7 @@
         <v>9074</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A144" s="1">
         <v>43994</v>
       </c>
@@ -12378,7 +12381,7 @@
         <v>112</v>
       </c>
       <c r="D144" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E144" t="s">
         <v>612</v>
@@ -12432,7 +12435,7 @@
         <v>9075</v>
       </c>
     </row>
-    <row r="145" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A145" s="1">
         <v>43994</v>
       </c>
@@ -12443,7 +12446,7 @@
         <v>112</v>
       </c>
       <c r="D145" t="s">
-        <v>695</v>
+        <v>736</v>
       </c>
       <c r="E145" t="s">
         <v>612</v>
@@ -12497,7 +12500,7 @@
         <v>9079</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A146" s="1">
         <v>43994</v>
       </c>
@@ -12508,7 +12511,7 @@
         <v>112</v>
       </c>
       <c r="D146" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="E146" t="s">
         <v>612</v>
@@ -12562,7 +12565,7 @@
         <v>9081</v>
       </c>
     </row>
-    <row r="147" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A147" s="1">
         <v>43994</v>
       </c>
@@ -12627,7 +12630,7 @@
         <v>9087</v>
       </c>
     </row>
-    <row r="148" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A148" s="1">
         <v>43994</v>
       </c>
@@ -12638,7 +12641,7 @@
         <v>112</v>
       </c>
       <c r="D148" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="E148" t="s">
         <v>612</v>
@@ -12692,7 +12695,7 @@
         <v>9091</v>
       </c>
     </row>
-    <row r="149" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A149" s="1">
         <v>43994</v>
       </c>
@@ -12703,7 +12706,7 @@
         <v>112</v>
       </c>
       <c r="D149" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E149" t="s">
         <v>612</v>
@@ -12757,7 +12760,7 @@
         <v>9092</v>
       </c>
     </row>
-    <row r="150" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A150" s="1">
         <v>43994</v>
       </c>
@@ -12768,7 +12771,7 @@
         <v>112</v>
       </c>
       <c r="D150" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="E150" t="s">
         <v>612</v>
@@ -12822,7 +12825,7 @@
         <v>9093</v>
       </c>
     </row>
-    <row r="151" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A151" s="1">
         <v>43994</v>
       </c>
@@ -12887,7 +12890,7 @@
         <v>9094</v>
       </c>
     </row>
-    <row r="152" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A152" s="1">
         <v>43994</v>
       </c>
@@ -12898,7 +12901,7 @@
         <v>112</v>
       </c>
       <c r="D152" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="E152" t="s">
         <v>612</v>
@@ -12952,7 +12955,7 @@
         <v>9096</v>
       </c>
     </row>
-    <row r="153" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A153" s="1">
         <v>43994</v>
       </c>
@@ -13017,7 +13020,7 @@
         <v>9098</v>
       </c>
     </row>
-    <row r="154" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A154" s="1">
         <v>44001</v>
       </c>
@@ -13028,7 +13031,7 @@
         <v>112</v>
       </c>
       <c r="D154" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E154" t="s">
         <v>612</v>
@@ -13082,7 +13085,7 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="155" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A155" s="1">
         <v>43994</v>
       </c>
@@ -13093,7 +13096,7 @@
         <v>112</v>
       </c>
       <c r="D155" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E155" t="s">
         <v>612</v>
@@ -13153,7 +13156,7 @@
         <v>9111</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A156" s="1">
         <v>43994</v>
       </c>
@@ -13164,7 +13167,7 @@
         <v>112</v>
       </c>
       <c r="D156" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E156" t="s">
         <v>612</v>
@@ -13224,7 +13227,7 @@
         <v>9113</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A157" s="1">
         <v>43994</v>
       </c>
@@ -13235,7 +13238,7 @@
         <v>112</v>
       </c>
       <c r="D157" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="E157" t="s">
         <v>612</v>
@@ -13289,7 +13292,7 @@
         <v>9117</v>
       </c>
     </row>
-    <row r="158" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A158" s="1">
         <v>43994</v>
       </c>
@@ -13300,7 +13303,7 @@
         <v>112</v>
       </c>
       <c r="D158" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="E158" t="s">
         <v>612</v>
@@ -13354,7 +13357,7 @@
         <v>9120</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A159" s="1">
         <v>43994</v>
       </c>
@@ -13365,7 +13368,7 @@
         <v>112</v>
       </c>
       <c r="D159" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E159" t="s">
         <v>612</v>
@@ -13419,7 +13422,7 @@
         <v>9121</v>
       </c>
     </row>
-    <row r="160" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A160" s="1">
         <v>43997</v>
       </c>
@@ -13430,7 +13433,7 @@
         <v>112</v>
       </c>
       <c r="D160" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="E160" t="s">
         <v>612</v>
@@ -13490,7 +13493,7 @@
         <v>9124</v>
       </c>
     </row>
-    <row r="161" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A161" s="1">
         <v>43994</v>
       </c>
@@ -13501,7 +13504,7 @@
         <v>112</v>
       </c>
       <c r="D161" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E161" t="s">
         <v>612</v>
@@ -13555,7 +13558,7 @@
         <v>9127</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A162" s="1">
         <v>43994</v>
       </c>
@@ -13566,7 +13569,7 @@
         <v>112</v>
       </c>
       <c r="D162" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E162" t="s">
         <v>612</v>
@@ -13620,7 +13623,7 @@
         <v>9129</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A163" s="1">
         <v>43994</v>
       </c>
@@ -13631,7 +13634,7 @@
         <v>112</v>
       </c>
       <c r="D163" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="E163" t="s">
         <v>612</v>
@@ -13691,7 +13694,7 @@
         <v>9133</v>
       </c>
     </row>
-    <row r="164" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A164" s="1">
         <v>43994</v>
       </c>
@@ -13702,7 +13705,7 @@
         <v>112</v>
       </c>
       <c r="D164" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="E164" t="s">
         <v>612</v>
@@ -13756,7 +13759,7 @@
         <v>9137</v>
       </c>
     </row>
-    <row r="165" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A165" s="1">
         <v>43994</v>
       </c>
@@ -13767,7 +13770,7 @@
         <v>112</v>
       </c>
       <c r="D165" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="E165" t="s">
         <v>612</v>
@@ -13827,7 +13830,7 @@
         <v>9138</v>
       </c>
     </row>
-    <row r="166" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A166" s="1">
         <v>47288</v>
       </c>
@@ -13838,7 +13841,7 @@
         <v>112</v>
       </c>
       <c r="D166" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E166" t="s">
         <v>612</v>
@@ -13892,7 +13895,7 @@
         <v>9149</v>
       </c>
     </row>
-    <row r="167" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A167" s="1">
         <v>43997</v>
       </c>
@@ -13903,7 +13906,7 @@
         <v>112</v>
       </c>
       <c r="D167" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E167" t="s">
         <v>612</v>
@@ -13963,7 +13966,7 @@
         <v>9150</v>
       </c>
     </row>
-    <row r="168" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A168" s="1">
         <v>44001</v>
       </c>
@@ -13974,7 +13977,7 @@
         <v>112</v>
       </c>
       <c r="D168" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E168" t="s">
         <v>612</v>
@@ -14028,7 +14031,7 @@
         <v>9152</v>
       </c>
     </row>
-    <row r="169" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A169" s="1">
         <v>44001</v>
       </c>
@@ -14039,7 +14042,7 @@
         <v>112</v>
       </c>
       <c r="D169" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E169" t="s">
         <v>612</v>
@@ -14093,7 +14096,7 @@
         <v>9156</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A170" s="1">
         <v>44009</v>
       </c>
@@ -14104,7 +14107,7 @@
         <v>112</v>
       </c>
       <c r="D170" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="E170" t="s">
         <v>612</v>
@@ -14164,7 +14167,7 @@
         <v>9157</v>
       </c>
     </row>
-    <row r="171" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A171" s="1">
         <v>44015</v>
       </c>
@@ -14175,7 +14178,7 @@
         <v>112</v>
       </c>
       <c r="D171" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="E171" t="s">
         <v>612</v>
@@ -14229,7 +14232,7 @@
         <v>9191</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A172" s="1">
         <v>44028</v>
       </c>
@@ -14240,7 +14243,7 @@
         <v>112</v>
       </c>
       <c r="D172" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="E172" t="s">
         <v>612</v>
@@ -14294,7 +14297,7 @@
         <v>9258</v>
       </c>
     </row>
-    <row r="173" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A173" s="1">
         <v>44029</v>
       </c>
@@ -14305,7 +14308,7 @@
         <v>112</v>
       </c>
       <c r="D173" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="E173" t="s">
         <v>612</v>
@@ -14359,7 +14362,7 @@
         <v>9276</v>
       </c>
     </row>
-    <row r="174" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A174" s="1">
         <v>44027</v>
       </c>
@@ -14424,7 +14427,7 @@
         <v>9280</v>
       </c>
     </row>
-    <row r="175" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A175" s="1">
         <v>44093</v>
       </c>
@@ -14513,7 +14516,7 @@
         <v>9351</v>
       </c>
     </row>
-    <row r="176" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A176" s="1">
         <v>44043</v>
       </c>
@@ -14578,7 +14581,7 @@
         <v>8873</v>
       </c>
     </row>
-    <row r="177" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A177" s="1">
         <v>44042</v>
       </c>
@@ -14661,7 +14664,7 @@
         <v>9158</v>
       </c>
     </row>
-    <row r="178" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A178" s="1">
         <v>44057</v>
       </c>
@@ -14750,7 +14753,7 @@
         <v>9201</v>
       </c>
     </row>
-    <row r="179" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A179" s="1">
         <v>44047</v>
       </c>
@@ -14839,7 +14842,7 @@
         <v>9296</v>
       </c>
     </row>
-    <row r="180" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A180" s="1">
         <v>44066</v>
       </c>
@@ -14928,7 +14931,7 @@
         <v>9327</v>
       </c>
     </row>
-    <row r="181" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A181" s="1">
         <v>44048</v>
       </c>
@@ -15020,7 +15023,7 @@
         <v>7987</v>
       </c>
     </row>
-    <row r="182" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A182" s="1">
         <v>44001</v>
       </c>
@@ -15085,7 +15088,7 @@
         <v>9029</v>
       </c>
     </row>
-    <row r="183" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A183" s="1">
         <v>44008</v>
       </c>
@@ -15150,7 +15153,7 @@
         <v>9031</v>
       </c>
     </row>
-    <row r="184" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A184" s="1">
         <v>44008</v>
       </c>
@@ -15161,7 +15164,7 @@
         <v>151</v>
       </c>
       <c r="D184" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E184" t="s">
         <v>612</v>
@@ -15221,7 +15224,7 @@
         <v>9080</v>
       </c>
     </row>
-    <row r="185" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A185" s="1">
         <v>44015</v>
       </c>
@@ -15232,7 +15235,7 @@
         <v>151</v>
       </c>
       <c r="D185" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="E185" t="s">
         <v>612</v>
@@ -15286,7 +15289,7 @@
         <v>9160</v>
       </c>
     </row>
-    <row r="186" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A186" s="1">
         <v>44015</v>
       </c>
@@ -15351,7 +15354,7 @@
         <v>9162</v>
       </c>
     </row>
-    <row r="187" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A187" s="1">
         <v>44015</v>
       </c>
@@ -15413,7 +15416,7 @@
         <v>9180</v>
       </c>
     </row>
-    <row r="188" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A188" s="1">
         <v>44015</v>
       </c>
@@ -15424,7 +15427,7 @@
         <v>151</v>
       </c>
       <c r="D188" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="E188" t="s">
         <v>612</v>
@@ -15469,7 +15472,7 @@
         <v>9182</v>
       </c>
     </row>
-    <row r="189" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A189" s="1">
         <v>44015</v>
       </c>
@@ -15480,7 +15483,7 @@
         <v>151</v>
       </c>
       <c r="D189" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="E189" t="s">
         <v>612</v>
@@ -15525,7 +15528,7 @@
         <v>9184</v>
       </c>
     </row>
-    <row r="190" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A190" s="1">
         <v>44015</v>
       </c>
@@ -15536,7 +15539,7 @@
         <v>151</v>
       </c>
       <c r="D190" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E190" t="s">
         <v>612</v>
@@ -15581,7 +15584,7 @@
         <v>9186</v>
       </c>
     </row>
-    <row r="191" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A191" s="1">
         <v>44015</v>
       </c>
@@ -15592,7 +15595,7 @@
         <v>151</v>
       </c>
       <c r="D191" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E191" t="s">
         <v>612</v>
@@ -15637,7 +15640,7 @@
         <v>9187</v>
       </c>
     </row>
-    <row r="192" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A192" s="1">
         <v>44015</v>
       </c>
@@ -15648,7 +15651,7 @@
         <v>151</v>
       </c>
       <c r="D192" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="E192" t="s">
         <v>612</v>
@@ -15702,7 +15705,7 @@
         <v>9188</v>
       </c>
     </row>
-    <row r="193" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A193" s="1">
         <v>44015</v>
       </c>
@@ -15767,7 +15770,7 @@
         <v>9193</v>
       </c>
     </row>
-    <row r="194" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A194" s="1">
         <v>44015</v>
       </c>
@@ -15832,7 +15835,7 @@
         <v>9194</v>
       </c>
     </row>
-    <row r="195" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A195" s="1">
         <v>44015</v>
       </c>
@@ -15843,7 +15846,7 @@
         <v>151</v>
       </c>
       <c r="D195" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E195" t="s">
         <v>612</v>
@@ -15897,7 +15900,7 @@
         <v>9195</v>
       </c>
     </row>
-    <row r="196" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A196" s="1">
         <v>44022</v>
       </c>
@@ -15908,7 +15911,7 @@
         <v>151</v>
       </c>
       <c r="D196" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E196" t="s">
         <v>612</v>
@@ -15962,7 +15965,7 @@
         <v>9242</v>
       </c>
     </row>
-    <row r="197" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A197" s="1">
         <v>44022</v>
       </c>
@@ -15973,7 +15976,7 @@
         <v>151</v>
       </c>
       <c r="D197" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E197" t="s">
         <v>612</v>
@@ -16027,7 +16030,7 @@
         <v>9257</v>
       </c>
     </row>
-    <row r="198" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A198" s="1">
         <v>44029</v>
       </c>
@@ -16092,7 +16095,7 @@
         <v>9267</v>
       </c>
     </row>
-    <row r="199" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A199" s="1">
         <v>44027</v>
       </c>
@@ -16157,7 +16160,7 @@
         <v>9281</v>
       </c>
     </row>
-    <row r="200" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A200" s="1">
         <v>44029</v>
       </c>
@@ -16168,7 +16171,7 @@
         <v>151</v>
       </c>
       <c r="D200" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E200" t="s">
         <v>612</v>
@@ -16222,7 +16225,7 @@
         <v>9283</v>
       </c>
     </row>
-    <row r="201" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A201" s="1">
         <v>44036</v>
       </c>
@@ -16233,7 +16236,7 @@
         <v>151</v>
       </c>
       <c r="D201" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E201" t="s">
         <v>612</v>
@@ -16287,7 +16290,7 @@
         <v>9313</v>
       </c>
     </row>
-    <row r="202" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A202" s="1">
         <v>44036</v>
       </c>
@@ -16298,7 +16301,7 @@
         <v>151</v>
       </c>
       <c r="D202" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="E202" t="s">
         <v>612</v>
@@ -16352,7 +16355,7 @@
         <v>9333</v>
       </c>
     </row>
-    <row r="203" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A203" s="1">
         <v>44149</v>
       </c>
@@ -16447,7 +16450,7 @@
         <v>7945</v>
       </c>
     </row>
-    <row r="204" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A204" s="1">
         <v>44036</v>
       </c>
@@ -16539,7 +16542,7 @@
         <v>9169</v>
       </c>
     </row>
-    <row r="205" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A205" s="1">
         <v>44050</v>
       </c>
@@ -16601,7 +16604,7 @@
         <v>9189</v>
       </c>
     </row>
-    <row r="206" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A206" s="1">
         <v>44050</v>
       </c>
@@ -16663,7 +16666,7 @@
         <v>9202</v>
       </c>
     </row>
-    <row r="207" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A207" s="1">
         <v>44050</v>
       </c>
@@ -16725,7 +16728,7 @@
         <v>9250</v>
       </c>
     </row>
-    <row r="208" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A208" s="1">
         <v>44089</v>
       </c>
@@ -16820,7 +16823,7 @@
         <v>9275</v>
       </c>
     </row>
-    <row r="209" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A209" s="1">
         <v>44050</v>
       </c>
@@ -16831,7 +16834,7 @@
         <v>388</v>
       </c>
       <c r="D209" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E209" t="s">
         <v>612</v>
@@ -16882,7 +16885,7 @@
         <v>9297</v>
       </c>
     </row>
-    <row r="210" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A210" s="1">
         <v>44050</v>
       </c>
@@ -16893,7 +16896,7 @@
         <v>388</v>
       </c>
       <c r="D210" t="s">
-        <v>720</v>
+        <v>737</v>
       </c>
       <c r="E210" t="s">
         <v>612</v>
@@ -16932,7 +16935,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="211" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A211" s="1">
         <v>44050</v>
       </c>
@@ -16997,7 +17000,7 @@
         <v>9301</v>
       </c>
     </row>
-    <row r="212" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A212" s="1">
         <v>44050</v>
       </c>
@@ -17059,7 +17062,7 @@
         <v>9304</v>
       </c>
     </row>
-    <row r="213" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A213" s="1">
         <v>44050</v>
       </c>
@@ -17070,7 +17073,7 @@
         <v>388</v>
       </c>
       <c r="D213" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="E213" t="s">
         <v>612</v>
@@ -17121,7 +17124,7 @@
         <v>9307</v>
       </c>
     </row>
-    <row r="214" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A214" s="1">
         <v>44050</v>
       </c>
@@ -17183,7 +17186,7 @@
         <v>9308</v>
       </c>
     </row>
-    <row r="215" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A215" s="1">
         <v>44050</v>
       </c>
@@ -17194,7 +17197,7 @@
         <v>388</v>
       </c>
       <c r="D215" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="E215" t="s">
         <v>612</v>
@@ -17245,7 +17248,7 @@
         <v>9310</v>
       </c>
     </row>
-    <row r="216" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A216" s="1">
         <v>44050</v>
       </c>
@@ -17256,7 +17259,7 @@
         <v>388</v>
       </c>
       <c r="D216" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E216" t="s">
         <v>612</v>
@@ -17307,7 +17310,7 @@
         <v>9315</v>
       </c>
     </row>
-    <row r="217" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A217" s="1">
         <v>44077</v>
       </c>
@@ -17399,7 +17402,7 @@
         <v>9317</v>
       </c>
     </row>
-    <row r="218" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A218" s="1">
         <v>44050</v>
       </c>
@@ -17410,7 +17413,7 @@
         <v>388</v>
       </c>
       <c r="D218" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E218" t="s">
         <v>612</v>
@@ -17461,7 +17464,7 @@
         <v>9320</v>
       </c>
     </row>
-    <row r="219" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A219" s="1">
         <v>44050</v>
       </c>
@@ -17472,7 +17475,7 @@
         <v>388</v>
       </c>
       <c r="D219" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E219" t="s">
         <v>612</v>
@@ -17523,7 +17526,7 @@
         <v>9321</v>
       </c>
     </row>
-    <row r="220" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A220" s="1">
         <v>44050</v>
       </c>
@@ -17585,7 +17588,7 @@
         <v>9325</v>
       </c>
     </row>
-    <row r="221" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A221" s="1">
         <v>44050</v>
       </c>
@@ -17596,7 +17599,7 @@
         <v>388</v>
       </c>
       <c r="D221" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="E221" t="s">
         <v>612</v>
@@ -17647,7 +17650,7 @@
         <v>9334</v>
       </c>
     </row>
-    <row r="222" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A222" s="1">
         <v>44050</v>
       </c>
@@ -17658,7 +17661,7 @@
         <v>388</v>
       </c>
       <c r="D222" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E222" t="s">
         <v>612</v>
@@ -17709,7 +17712,7 @@
         <v>9335</v>
       </c>
     </row>
-    <row r="223" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A223" s="1">
         <v>44050</v>
       </c>
@@ -17720,7 +17723,7 @@
         <v>388</v>
       </c>
       <c r="D223" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E223" t="s">
         <v>612</v>
@@ -17771,7 +17774,7 @@
         <v>9340</v>
       </c>
     </row>
-    <row r="224" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A224" s="1">
         <v>44302</v>
       </c>
@@ -17860,7 +17863,7 @@
         <v>9054</v>
       </c>
     </row>
-    <row r="225" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A225" s="1">
         <v>43994</v>
       </c>
@@ -17871,7 +17874,7 @@
         <v>285</v>
       </c>
       <c r="D225" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E225" t="s">
         <v>612</v>
@@ -17931,7 +17934,7 @@
         <v>9112</v>
       </c>
     </row>
-    <row r="226" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A226" s="1">
         <v>43994</v>
       </c>
@@ -17942,7 +17945,7 @@
         <v>285</v>
       </c>
       <c r="D226" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="E226" t="s">
         <v>612</v>
@@ -18002,7 +18005,7 @@
         <v>9114</v>
       </c>
     </row>
-    <row r="227" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A227" s="1">
         <v>44043</v>
       </c>
@@ -18013,7 +18016,7 @@
         <v>285</v>
       </c>
       <c r="D227" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E227" t="s">
         <v>612</v>
@@ -18067,7 +18070,7 @@
         <v>9343</v>
       </c>
     </row>
-    <row r="228" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A228" s="1">
         <v>44089</v>
       </c>
@@ -18162,7 +18165,7 @@
         <v>9274</v>
       </c>
     </row>
-    <row r="229" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A229" s="1">
         <v>44146</v>
       </c>
@@ -18257,7 +18260,7 @@
         <v>7946</v>
       </c>
     </row>
-    <row r="230" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A230" s="1">
         <v>43994</v>
       </c>
@@ -18322,7 +18325,7 @@
         <v>9027</v>
       </c>
     </row>
-    <row r="231" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A231" s="1">
         <v>44015</v>
       </c>
@@ -18333,7 +18336,7 @@
         <v>143</v>
       </c>
       <c r="D231" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="E231" t="s">
         <v>612</v>
@@ -18387,7 +18390,7 @@
         <v>9190</v>
       </c>
     </row>
-    <row r="232" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A232" s="1">
         <v>44029</v>
       </c>
@@ -18398,7 +18401,7 @@
         <v>143</v>
       </c>
       <c r="D232" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E232" t="s">
         <v>612</v>
@@ -18452,7 +18455,7 @@
         <v>9294</v>
       </c>
     </row>
-    <row r="233" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A233" s="1">
         <v>44044</v>
       </c>
@@ -18463,7 +18466,7 @@
         <v>510</v>
       </c>
       <c r="D233" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E233" t="s">
         <v>612</v>
@@ -18520,7 +18523,7 @@
         <v>9291</v>
       </c>
     </row>
-    <row r="234" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A234" s="1">
         <v>44092</v>
       </c>
@@ -18585,7 +18588,7 @@
         <v>9105</v>
       </c>
     </row>
-    <row r="235" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A235" s="1">
         <v>44006</v>
       </c>
@@ -18596,7 +18599,7 @@
         <v>401</v>
       </c>
       <c r="D235" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="E235" t="s">
         <v>612</v>
@@ -18641,7 +18644,7 @@
         <v>9173</v>
       </c>
     </row>
-    <row r="236" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A236" s="1">
         <v>43994</v>
       </c>
@@ -18706,7 +18709,7 @@
         <v>9028</v>
       </c>
     </row>
-    <row r="237" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A237" s="1">
         <v>44001</v>
       </c>
@@ -18717,7 +18720,7 @@
         <v>145</v>
       </c>
       <c r="D237" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E237" t="s">
         <v>612</v>
@@ -18771,7 +18774,7 @@
         <v>9103</v>
       </c>
     </row>
-    <row r="238" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A238" s="1">
         <v>44001</v>
       </c>
@@ -18836,7 +18839,7 @@
         <v>9115</v>
       </c>
     </row>
-    <row r="239" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A239" s="1">
         <v>44001</v>
       </c>
@@ -18847,7 +18850,7 @@
         <v>145</v>
       </c>
       <c r="D239" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E239" t="s">
         <v>612</v>
@@ -18901,7 +18904,7 @@
         <v>9116</v>
       </c>
     </row>
-    <row r="240" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A240" s="1">
         <v>44001</v>
       </c>
@@ -18912,7 +18915,7 @@
         <v>145</v>
       </c>
       <c r="D240" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E240" t="s">
         <v>612</v>
@@ -18972,7 +18975,7 @@
         <v>9118</v>
       </c>
     </row>
-    <row r="241" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A241" s="1">
         <v>44001</v>
       </c>
@@ -18983,7 +18986,7 @@
         <v>145</v>
       </c>
       <c r="D241" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E241" t="s">
         <v>612</v>
@@ -19037,7 +19040,7 @@
         <v>9122</v>
       </c>
     </row>
-    <row r="242" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A242" s="1">
         <v>44001</v>
       </c>
@@ -19048,7 +19051,7 @@
         <v>145</v>
       </c>
       <c r="D242" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E242" t="s">
         <v>612</v>
@@ -19102,7 +19105,7 @@
         <v>9123</v>
       </c>
     </row>
-    <row r="243" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A243" s="1">
         <v>44001</v>
       </c>
@@ -19113,7 +19116,7 @@
         <v>145</v>
       </c>
       <c r="D243" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E243" t="s">
         <v>612</v>
@@ -19167,7 +19170,7 @@
         <v>9130</v>
       </c>
     </row>
-    <row r="244" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A244" s="1">
         <v>44011</v>
       </c>
@@ -19178,7 +19181,7 @@
         <v>145</v>
       </c>
       <c r="D244" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="E244" t="s">
         <v>612</v>
@@ -19232,7 +19235,7 @@
         <v>9131</v>
       </c>
     </row>
-    <row r="245" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A245" s="1">
         <v>44001</v>
       </c>
@@ -19243,7 +19246,7 @@
         <v>145</v>
       </c>
       <c r="D245" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="E245" t="s">
         <v>612</v>
@@ -19297,7 +19300,7 @@
         <v>9134</v>
       </c>
     </row>
-    <row r="246" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A246" s="1">
         <v>44001</v>
       </c>
@@ -19308,7 +19311,7 @@
         <v>145</v>
       </c>
       <c r="D246" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="E246" t="s">
         <v>612</v>
@@ -19362,7 +19365,7 @@
         <v>9135</v>
       </c>
     </row>
-    <row r="247" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A247" s="1">
         <v>44001</v>
       </c>
@@ -19373,7 +19376,7 @@
         <v>145</v>
       </c>
       <c r="D247" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E247" t="s">
         <v>612</v>
@@ -19427,7 +19430,7 @@
         <v>9140</v>
       </c>
     </row>
-    <row r="248" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A248" s="1">
         <v>44001</v>
       </c>
@@ -19438,7 +19441,7 @@
         <v>145</v>
       </c>
       <c r="D248" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="E248" t="s">
         <v>612</v>
@@ -19492,7 +19495,7 @@
         <v>9141</v>
       </c>
     </row>
-    <row r="249" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A249" s="1">
         <v>44001</v>
       </c>
@@ -19503,7 +19506,7 @@
         <v>145</v>
       </c>
       <c r="D249" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="E249" t="s">
         <v>612</v>
@@ -19563,7 +19566,7 @@
         <v>9143</v>
       </c>
     </row>
-    <row r="250" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A250" s="1">
         <v>44001</v>
       </c>
@@ -19574,7 +19577,7 @@
         <v>145</v>
       </c>
       <c r="D250" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="E250" t="s">
         <v>612</v>
@@ -19628,7 +19631,7 @@
         <v>9148</v>
       </c>
     </row>
-    <row r="251" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A251" s="1">
         <v>44001</v>
       </c>
@@ -19693,7 +19696,7 @@
         <v>9151</v>
       </c>
     </row>
-    <row r="252" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A252" s="1">
         <v>44001</v>
       </c>
@@ -19704,7 +19707,7 @@
         <v>145</v>
       </c>
       <c r="D252" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E252" t="s">
         <v>612</v>
@@ -19758,7 +19761,7 @@
         <v>9153</v>
       </c>
     </row>
-    <row r="253" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A253" s="1">
         <v>44001</v>
       </c>
@@ -19769,7 +19772,7 @@
         <v>145</v>
       </c>
       <c r="D253" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="E253" t="s">
         <v>612</v>
@@ -19823,7 +19826,7 @@
         <v>9154</v>
       </c>
     </row>
-    <row r="254" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A254" s="1">
         <v>44022</v>
       </c>
@@ -19834,7 +19837,7 @@
         <v>145</v>
       </c>
       <c r="D254" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="E254" t="s">
         <v>612</v>
@@ -19888,7 +19891,7 @@
         <v>9161</v>
       </c>
     </row>
-    <row r="255" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A255" s="1">
         <v>44001</v>
       </c>
@@ -19950,7 +19953,7 @@
         <v>9170</v>
       </c>
     </row>
-    <row r="256" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A256" s="1">
         <v>44001</v>
       </c>
@@ -19961,7 +19964,7 @@
         <v>145</v>
       </c>
       <c r="D256" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E256" t="s">
         <v>612</v>
@@ -20006,7 +20009,7 @@
         <v>9171</v>
       </c>
     </row>
-    <row r="257" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A257" s="1">
         <v>44001</v>
       </c>
@@ -20017,7 +20020,7 @@
         <v>145</v>
       </c>
       <c r="D257" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E257" t="s">
         <v>612</v>
@@ -20062,7 +20065,7 @@
         <v>9172</v>
       </c>
     </row>
-    <row r="258" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A258" s="1">
         <v>44008</v>
       </c>
@@ -20073,7 +20076,7 @@
         <v>145</v>
       </c>
       <c r="D258" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E258" t="s">
         <v>612</v>
@@ -20118,7 +20121,7 @@
         <v>9175</v>
       </c>
     </row>
-    <row r="259" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A259" s="1">
         <v>44008</v>
       </c>
@@ -20129,7 +20132,7 @@
         <v>145</v>
       </c>
       <c r="D259" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E259" t="s">
         <v>612</v>
@@ -20174,7 +20177,7 @@
         <v>9177</v>
       </c>
     </row>
-    <row r="260" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A260" s="1">
         <v>44008</v>
       </c>
@@ -20236,7 +20239,7 @@
         <v>9179</v>
       </c>
     </row>
-    <row r="261" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A261" s="1">
         <v>44015</v>
       </c>
@@ -20247,7 +20250,7 @@
         <v>145</v>
       </c>
       <c r="D261" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E261" t="s">
         <v>612</v>
@@ -20301,7 +20304,7 @@
         <v>9196</v>
       </c>
     </row>
-    <row r="262" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A262" s="1">
         <v>44022</v>
       </c>
@@ -20366,7 +20369,7 @@
         <v>9208</v>
       </c>
     </row>
-    <row r="263" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A263" s="1">
         <v>44028</v>
       </c>
@@ -20377,7 +20380,7 @@
         <v>145</v>
       </c>
       <c r="D263" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="E263" t="s">
         <v>612</v>
@@ -20431,7 +20434,7 @@
         <v>9259</v>
       </c>
     </row>
-    <row r="264" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A264" s="1">
         <v>44029</v>
       </c>
@@ -20442,7 +20445,7 @@
         <v>145</v>
       </c>
       <c r="D264" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="E264" t="s">
         <v>612</v>
@@ -20496,7 +20499,7 @@
         <v>9286</v>
       </c>
     </row>
-    <row r="265" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A265" s="1">
         <v>44027</v>
       </c>
@@ -20507,7 +20510,7 @@
         <v>145</v>
       </c>
       <c r="D265" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="E265" t="s">
         <v>612</v>
@@ -20561,7 +20564,7 @@
         <v>9287</v>
       </c>
     </row>
-    <row r="266" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A266" s="1">
         <v>44041</v>
       </c>
@@ -20572,7 +20575,7 @@
         <v>145</v>
       </c>
       <c r="D266" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E266" t="s">
         <v>612</v>
@@ -20626,7 +20629,7 @@
         <v>9331</v>
       </c>
     </row>
-    <row r="267" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A267" s="1">
         <v>44083</v>
       </c>
@@ -20718,7 +20721,7 @@
         <v>9330</v>
       </c>
     </row>
-    <row r="268" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A268" s="1">
         <v>43980</v>
       </c>
@@ -20729,7 +20732,7 @@
         <v>121</v>
       </c>
       <c r="D268" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="E268" t="s">
         <v>612</v>
@@ -20789,7 +20792,7 @@
         <v>9017</v>
       </c>
     </row>
-    <row r="269" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A269" s="1">
         <v>44001</v>
       </c>
@@ -20800,7 +20803,7 @@
         <v>121</v>
       </c>
       <c r="D269" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="E269" t="s">
         <v>612</v>
@@ -20857,7 +20860,7 @@
         <v>9139</v>
       </c>
     </row>
-    <row r="270" spans="1:36" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:36" x14ac:dyDescent="0.15">
       <c r="A270" s="1">
         <v>44022</v>
       </c>
@@ -20868,7 +20871,7 @@
         <v>121</v>
       </c>
       <c r="D270" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E270" t="s">
         <v>612</v>

</xml_diff>